<commit_message>
Adds a great deal of things - Sidebar interaaction is bugged
</commit_message>
<xml_diff>
--- a/Test_Print_Data.xlsx
+++ b/Test_Print_Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\niko\PrusaSlicerSource\PrusaSlicer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7866A8C5-E484-4B4E-B949-3C29CC5A7894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{217AAD7A-2C7B-44A2-AAE5-EDFA692BD6BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F15533C0-FC78-4CA7-8F95-E34C347E1025}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="2400" windowHeight="585" xr2:uid="{F15533C0-FC78-4CA7-8F95-E34C347E1025}"/>
   </bookViews>
   <sheets>
     <sheet name="LW-PLA Single Wall Test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,10 +99,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -141,6 +143,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,6 +183,504 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>1x Extrusion</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'LW-PLA Single Wall Test'!$B$1:$O$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>260</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'LW-PLA Single Wall Test'!$B$3:$O$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-24FF-46EA-96D2-7EBFDB825DAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1767918672"/>
+        <c:axId val="1428032208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1767918672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Hotend temperature in degrees Celsius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1428032208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1428032208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Wall thiuckness in mm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1767918672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -193,7 +695,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-AT"/>
-              <a:t>1x Extrusion</a:t>
+              <a:t>0,45 Wall Thickness</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -301,51 +803,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'LW-PLA Single Wall Test'!$B$3:$O$3</c:f>
+              <c:f>'LW-PLA Single Wall Test'!$B$8:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.47</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.73</c:v>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.89</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.91</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.95</c:v>
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>0.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -353,7 +855,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-24FF-46EA-96D2-7EBFDB825DAF}"/>
+              <c16:uniqueId val="{00000000-483C-42FC-9707-BAED349BBA90}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -366,11 +868,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1767918672"/>
-        <c:axId val="1428032208"/>
+        <c:axId val="1621876335"/>
+        <c:axId val="1629580255"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1767918672"/>
+        <c:axId val="1621876335"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -413,7 +915,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1428032208"/>
+        <c:crossAx val="1629580255"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -421,10 +923,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1428032208"/>
+        <c:axId val="1629580255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -473,7 +974,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1767918672"/>
+        <c:crossAx val="1621876335"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -562,7 +1063,560 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="237">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="rnd"/>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1111,6 +2165,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4958F3BC-29DE-4CED-BBD2-45EC3DFA7B9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1443,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E69DC0A-E22A-4C53-8E6F-57F327EBFBF9}">
   <dimension ref="A1:AC24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,9 +2760,11 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>0.47</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.51</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1691,10 +2783,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="4">
-        <v>0.82</v>
+        <v>0.75</v>
       </c>
       <c r="G6" s="4">
-        <v>0.71</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H6" s="4">
         <v>0.59</v>
@@ -1733,7 +2825,9 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>0.49</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1763,10 +2857,37 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>0.93</v>
+        <v>0.92</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.38</v>
       </c>
       <c r="J8" s="6">
         <v>0.37</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0.32</v>
       </c>
       <c r="P8" s="1"/>
     </row>
@@ -1786,7 +2907,9 @@
       <c r="E9" s="3">
         <v>0.45</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <v>0.45</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>

</xml_diff>